<commit_message>
Mejoras de compilación metodo buscar rut y se añade total con size para mostar total en los metodos listar
</commit_message>
<xml_diff>
--- a/src/main/resources/SalmonttListas.xlsx
+++ b/src/main/resources/SalmonttListas.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\IdeaProjects\SumativaExp2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD9C392-2A52-4726-A467-FDABC9D5F9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD36B38-CC75-46CD-BC8F-6E0690BBDDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4A0AC0AF-66C9-4A8D-A91F-20F5A6C8B6FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A0AC0AF-66C9-4A8D-A91F-20F5A6C8B6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Proveedores" sheetId="1" r:id="rId1"/>
     <sheet name="Clientes" sheetId="2" r:id="rId2"/>
     <sheet name="Trabajadores" sheetId="3" r:id="rId3"/>
-    <sheet name="CentroCultivo" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1298,7 +1297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EE65FB-178C-45A6-902D-39B02B5C8D19}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1541,7 +1540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898AA76D-4C8F-43D3-AECB-551ED8FD72E4}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1885,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB6406D-C12C-4555-8563-D6F997F093D9}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2616,18 +2615,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E7FC82-B044-404F-8DFD-A26F992EE49C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>